<commit_message>
committing from Surface borom
</commit_message>
<xml_diff>
--- a/Excel Modelos FAB.xlsx
+++ b/Excel Modelos FAB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2131239_cognizant_com/Documents/Desktop/Repo Pepsico Market Share/proc_doc/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2131239_cognizant_com/Documents/Desktop/Repo Pepsico Market Share/proc_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_EE6034CB930250D18AA0A26AEBD8C78B9F568004" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ECBF5E5-F67E-4928-9321-DDA6094DC277}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_EE6034CB930250D18AA0A26AEBD8C78B9F568004" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5D403A1-60E3-4DA4-A5B5-F06E705E7087}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2265" yWindow="4215" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>NUMERO_A</t>
   </si>
@@ -140,13 +140,25 @@
   </si>
   <si>
     <t>CORREO_ARBITRO</t>
+  </si>
+  <si>
+    <t>Juan Perez</t>
+  </si>
+  <si>
+    <t>juan.perez@gmail.com</t>
+  </si>
+  <si>
+    <t>Jose Garcia</t>
+  </si>
+  <si>
+    <t>jose.garcia@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +178,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,10 +212,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -204,8 +225,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -219,10 +242,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,10 +532,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +691,25 @@
         <v>38</v>
       </c>
     </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{035FE52D-4C36-4256-A6C5-F32FBE83B337}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{43525EA0-F400-4D0F-8EA3-9668D8CF4509}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>